<commit_message>
klasa person i csvreader dla niej
</commit_message>
<xml_diff>
--- a/test_files/dane_testowe_orange.xlsx
+++ b/test_files/dane_testowe_orange.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28526"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26327"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\GIT FILES\orange-scheduler\test_files\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\tajbe\Desktop\vs2022\java projekty\orange-scheduler\test_files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{14EAF58C-F672-4BE6-9228-F9C19F3AFD77}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{20EE29A0-F586-43F8-9027-F1FF50680F2C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-38520" yWindow="-3375" windowWidth="38640" windowHeight="21240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17520" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Arkusz1" sheetId="1" r:id="rId1"/>
@@ -125,7 +125,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="mm\.dd"/>
   </numFmts>
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -137,10 +137,6 @@
       <color theme="1"/>
       <name val="Arial"/>
       <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="Arial"/>
     </font>
   </fonts>
   <fills count="4">
@@ -163,7 +159,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="4">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -199,31 +195,16 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color rgb="FF000000"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF000000"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF000000"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="20" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="1" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -463,26 +444,26 @@
       <c r="D1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="E1" s="3"/>
-      <c r="F1" s="4"/>
-      <c r="G1" s="5" t="s">
+      <c r="E1" s="1"/>
+      <c r="F1" s="3"/>
+      <c r="G1" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="H1" s="5" t="s">
-        <v>2</v>
-      </c>
-      <c r="I1" s="5"/>
-      <c r="J1" s="5"/>
-      <c r="K1" s="5"/>
-      <c r="L1" s="5"/>
-      <c r="M1" s="5"/>
-      <c r="N1" s="5"/>
-      <c r="O1" s="5"/>
-      <c r="P1" s="5"/>
-      <c r="Q1" s="5"/>
-      <c r="R1" s="5"/>
-      <c r="S1" s="5"/>
-      <c r="T1" s="5"/>
+      <c r="H1" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="I1" s="3"/>
+      <c r="J1" s="3"/>
+      <c r="K1" s="3"/>
+      <c r="L1" s="3"/>
+      <c r="M1" s="3"/>
+      <c r="N1" s="3"/>
+      <c r="O1" s="3"/>
+      <c r="P1" s="3"/>
+      <c r="Q1" s="3"/>
+      <c r="R1" s="3"/>
+      <c r="S1" s="3"/>
+      <c r="T1" s="3"/>
     </row>
     <row r="2" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
@@ -500,47 +481,47 @@
       <c r="E2" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F2" s="4"/>
-      <c r="G2" s="5">
+      <c r="F2" s="3"/>
+      <c r="G2" s="3">
         <v>6</v>
       </c>
-      <c r="H2" s="5">
+      <c r="H2" s="3">
         <v>7</v>
       </c>
-      <c r="I2" s="5">
+      <c r="I2" s="3">
         <v>8</v>
       </c>
-      <c r="J2" s="5">
+      <c r="J2" s="3">
         <v>9</v>
       </c>
-      <c r="K2" s="5">
+      <c r="K2" s="3">
         <v>10</v>
       </c>
-      <c r="L2" s="5">
+      <c r="L2" s="3">
         <v>11</v>
       </c>
-      <c r="M2" s="5">
+      <c r="M2" s="3">
         <v>12</v>
       </c>
-      <c r="N2" s="5">
+      <c r="N2" s="3">
         <v>13</v>
       </c>
-      <c r="O2" s="5">
+      <c r="O2" s="3">
         <v>14</v>
       </c>
-      <c r="P2" s="5">
+      <c r="P2" s="3">
         <v>15</v>
       </c>
-      <c r="Q2" s="5">
+      <c r="Q2" s="3">
         <v>16</v>
       </c>
-      <c r="R2" s="5">
+      <c r="R2" s="3">
         <v>17</v>
       </c>
-      <c r="S2" s="5">
+      <c r="S2" s="3">
         <v>18</v>
       </c>
-      <c r="T2" s="5">
+      <c r="T2" s="3">
         <v>19</v>
       </c>
     </row>
@@ -554,55 +535,55 @@
       <c r="C3" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D3" s="6">
+      <c r="D3" s="4">
         <v>0.33333333333333331</v>
       </c>
-      <c r="E3" s="6">
+      <c r="E3" s="4">
         <v>0.66666666666666663</v>
       </c>
-      <c r="F3" s="7">
+      <c r="F3" s="5">
         <v>45661</v>
       </c>
-      <c r="G3" s="5">
+      <c r="G3" s="3">
         <v>-1</v>
       </c>
-      <c r="H3" s="5">
+      <c r="H3" s="3">
         <v>-2</v>
       </c>
-      <c r="I3" s="5">
+      <c r="I3" s="3">
         <v>-3</v>
       </c>
-      <c r="J3" s="5">
+      <c r="J3" s="3">
         <v>-4</v>
       </c>
-      <c r="K3" s="5">
+      <c r="K3" s="3">
         <v>-4</v>
       </c>
-      <c r="L3" s="5">
+      <c r="L3" s="3">
         <v>-4</v>
       </c>
-      <c r="M3" s="5">
+      <c r="M3" s="3">
         <v>-4</v>
       </c>
-      <c r="N3" s="5">
+      <c r="N3" s="3">
         <v>-4</v>
       </c>
-      <c r="O3" s="5">
+      <c r="O3" s="3">
         <v>-4</v>
       </c>
-      <c r="P3" s="5">
+      <c r="P3" s="3">
         <v>-4</v>
       </c>
-      <c r="Q3" s="5">
+      <c r="Q3" s="3">
         <v>-4</v>
       </c>
-      <c r="R3" s="5">
+      <c r="R3" s="3">
         <v>-3</v>
       </c>
-      <c r="S3" s="5">
+      <c r="S3" s="3">
         <v>-2</v>
       </c>
-      <c r="T3" s="5">
+      <c r="T3" s="3">
         <v>-1</v>
       </c>
     </row>
@@ -616,31 +597,31 @@
       <c r="C4" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D4" s="6">
-        <v>0.25</v>
-      </c>
-      <c r="E4" s="6">
-        <v>0.83333333333333337</v>
-      </c>
-      <c r="F4" s="4"/>
-      <c r="G4" s="5" t="s">
+      <c r="D4" s="4">
+        <v>0.25</v>
+      </c>
+      <c r="E4" s="4">
+        <v>0.83333333333333337</v>
+      </c>
+      <c r="F4" s="3"/>
+      <c r="G4" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="H4" s="5" t="s">
+      <c r="H4" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="I4" s="5"/>
-      <c r="J4" s="5"/>
-      <c r="K4" s="5"/>
-      <c r="L4" s="5"/>
-      <c r="M4" s="5"/>
-      <c r="N4" s="5"/>
-      <c r="O4" s="5"/>
-      <c r="P4" s="5"/>
-      <c r="Q4" s="5"/>
-      <c r="R4" s="5"/>
-      <c r="S4" s="5"/>
-      <c r="T4" s="5"/>
+      <c r="I4" s="3"/>
+      <c r="J4" s="3"/>
+      <c r="K4" s="3"/>
+      <c r="L4" s="3"/>
+      <c r="M4" s="3"/>
+      <c r="N4" s="3"/>
+      <c r="O4" s="3"/>
+      <c r="P4" s="3"/>
+      <c r="Q4" s="3"/>
+      <c r="R4" s="3"/>
+      <c r="S4" s="3"/>
+      <c r="T4" s="3"/>
     </row>
     <row r="5" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A5" s="1">
@@ -652,53 +633,53 @@
       <c r="C5" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="D5" s="6">
-        <v>0.25</v>
-      </c>
-      <c r="E5" s="6">
-        <v>0.83333333333333337</v>
-      </c>
-      <c r="F5" s="4"/>
-      <c r="G5" s="5">
+      <c r="D5" s="4">
+        <v>0.25</v>
+      </c>
+      <c r="E5" s="4">
+        <v>0.83333333333333337</v>
+      </c>
+      <c r="F5" s="3"/>
+      <c r="G5" s="3">
         <v>6</v>
       </c>
-      <c r="H5" s="5">
+      <c r="H5" s="3">
         <v>7</v>
       </c>
-      <c r="I5" s="5">
+      <c r="I5" s="3">
         <v>8</v>
       </c>
-      <c r="J5" s="5">
+      <c r="J5" s="3">
         <v>9</v>
       </c>
-      <c r="K5" s="5">
+      <c r="K5" s="3">
         <v>10</v>
       </c>
-      <c r="L5" s="5">
+      <c r="L5" s="3">
         <v>11</v>
       </c>
-      <c r="M5" s="5">
+      <c r="M5" s="3">
         <v>12</v>
       </c>
-      <c r="N5" s="5">
+      <c r="N5" s="3">
         <v>13</v>
       </c>
-      <c r="O5" s="5">
+      <c r="O5" s="3">
         <v>14</v>
       </c>
-      <c r="P5" s="5">
+      <c r="P5" s="3">
         <v>15</v>
       </c>
-      <c r="Q5" s="5">
+      <c r="Q5" s="3">
         <v>16</v>
       </c>
-      <c r="R5" s="5">
+      <c r="R5" s="3">
         <v>17</v>
       </c>
-      <c r="S5" s="5">
+      <c r="S5" s="3">
         <v>18</v>
       </c>
-      <c r="T5" s="5">
+      <c r="T5" s="3">
         <v>19</v>
       </c>
     </row>
@@ -712,55 +693,55 @@
       <c r="C6" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="D6" s="6">
+      <c r="D6" s="4">
         <v>0.29166666666666669</v>
       </c>
-      <c r="E6" s="6">
+      <c r="E6" s="4">
         <v>0.54166666666666663</v>
       </c>
-      <c r="F6" s="7">
+      <c r="F6" s="5">
         <v>45661</v>
       </c>
-      <c r="G6" s="5">
+      <c r="G6" s="3">
         <v>-1</v>
       </c>
-      <c r="H6" s="5">
+      <c r="H6" s="3">
         <v>-1</v>
       </c>
-      <c r="I6" s="5">
+      <c r="I6" s="3">
         <v>-1</v>
       </c>
-      <c r="J6" s="5">
+      <c r="J6" s="3">
         <v>-1</v>
       </c>
-      <c r="K6" s="5">
+      <c r="K6" s="3">
         <v>-1</v>
       </c>
-      <c r="L6" s="5">
+      <c r="L6" s="3">
         <v>-2</v>
       </c>
-      <c r="M6" s="5">
+      <c r="M6" s="3">
         <v>-2</v>
       </c>
-      <c r="N6" s="5">
+      <c r="N6" s="3">
         <v>-2</v>
       </c>
-      <c r="O6" s="5">
+      <c r="O6" s="3">
         <v>-2</v>
       </c>
-      <c r="P6" s="5">
+      <c r="P6" s="3">
         <v>-2</v>
       </c>
-      <c r="Q6" s="5">
+      <c r="Q6" s="3">
         <v>-2</v>
       </c>
-      <c r="R6" s="5">
+      <c r="R6" s="3">
         <v>-2</v>
       </c>
-      <c r="S6" s="5">
+      <c r="S6" s="3">
         <v>-2</v>
       </c>
-      <c r="T6" s="5">
+      <c r="T6" s="3">
         <v>-2</v>
       </c>
     </row>
@@ -774,10 +755,10 @@
       <c r="C7" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D7" s="6">
+      <c r="D7" s="4">
         <v>0.41666666666666669</v>
       </c>
-      <c r="E7" s="6">
+      <c r="E7" s="4">
         <v>0.5</v>
       </c>
     </row>
@@ -791,10 +772,10 @@
       <c r="C8" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="D8" s="6">
+      <c r="D8" s="4">
         <v>0.33333333333333331</v>
       </c>
-      <c r="E8" s="6">
+      <c r="E8" s="4">
         <v>0.66666666666666663</v>
       </c>
     </row>
@@ -808,10 +789,10 @@
       <c r="C9" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="D9" s="6">
-        <v>0.25</v>
-      </c>
-      <c r="E9" s="6">
+      <c r="D9" s="4">
+        <v>0.25</v>
+      </c>
+      <c r="E9" s="4">
         <v>0.83333333333333337</v>
       </c>
     </row>
@@ -825,10 +806,10 @@
       <c r="C10" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D10" s="6">
-        <v>0.25</v>
-      </c>
-      <c r="E10" s="6">
+      <c r="D10" s="4">
+        <v>0.25</v>
+      </c>
+      <c r="E10" s="4">
         <v>0.83333333333333337</v>
       </c>
     </row>
@@ -842,10 +823,10 @@
       <c r="C11" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="D11" s="6">
-        <v>0.25</v>
-      </c>
-      <c r="E11" s="6">
+      <c r="D11" s="4">
+        <v>0.25</v>
+      </c>
+      <c r="E11" s="4">
         <v>0.83333333333333337</v>
       </c>
     </row>
@@ -859,10 +840,10 @@
       <c r="C12" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D12" s="6">
+      <c r="D12" s="4">
         <v>0.33333333333333331</v>
       </c>
-      <c r="E12" s="6">
+      <c r="E12" s="4">
         <v>0.66666666666666663</v>
       </c>
     </row>
@@ -876,10 +857,10 @@
       <c r="C13" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D13" s="6">
-        <v>0.25</v>
-      </c>
-      <c r="E13" s="6">
+      <c r="D13" s="4">
+        <v>0.25</v>
+      </c>
+      <c r="E13" s="4">
         <v>0.83333333333333337</v>
       </c>
     </row>
@@ -893,10 +874,10 @@
       <c r="C14" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="D14" s="6">
-        <v>0.25</v>
-      </c>
-      <c r="E14" s="6">
+      <c r="D14" s="4">
+        <v>0.25</v>
+      </c>
+      <c r="E14" s="4">
         <v>0.83333333333333337</v>
       </c>
     </row>
@@ -910,10 +891,10 @@
       <c r="C15" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="D15" s="6">
-        <v>0.25</v>
-      </c>
-      <c r="E15" s="6">
+      <c r="D15" s="4">
+        <v>0.25</v>
+      </c>
+      <c r="E15" s="4">
         <v>0.83333333333333337</v>
       </c>
     </row>
@@ -927,10 +908,10 @@
       <c r="C16" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D16" s="6">
+      <c r="D16" s="4">
         <v>0.41666666666666669</v>
       </c>
-      <c r="E16" s="6">
+      <c r="E16" s="4">
         <v>0.5</v>
       </c>
     </row>
@@ -944,10 +925,10 @@
       <c r="C17" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="D17" s="6">
-        <v>0.25</v>
-      </c>
-      <c r="E17" s="6">
+      <c r="D17" s="4">
+        <v>0.25</v>
+      </c>
+      <c r="E17" s="4">
         <v>0.83333333333333337</v>
       </c>
     </row>
@@ -961,10 +942,10 @@
       <c r="C18" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="D18" s="6">
-        <v>0.25</v>
-      </c>
-      <c r="E18" s="6">
+      <c r="D18" s="4">
+        <v>0.25</v>
+      </c>
+      <c r="E18" s="4">
         <v>0.83333333333333337</v>
       </c>
     </row>
@@ -978,10 +959,10 @@
       <c r="C19" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D19" s="6">
-        <v>0.25</v>
-      </c>
-      <c r="E19" s="6">
+      <c r="D19" s="4">
+        <v>0.25</v>
+      </c>
+      <c r="E19" s="4">
         <v>0.83333333333333337</v>
       </c>
     </row>
@@ -995,10 +976,10 @@
       <c r="C20" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="D20" s="6">
-        <v>0.25</v>
-      </c>
-      <c r="E20" s="6">
+      <c r="D20" s="4">
+        <v>0.25</v>
+      </c>
+      <c r="E20" s="4">
         <v>0.83333333333333337</v>
       </c>
     </row>
@@ -1012,10 +993,10 @@
       <c r="C21" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D21" s="6">
+      <c r="D21" s="4">
         <v>0.33333333333333331</v>
       </c>
-      <c r="E21" s="6">
+      <c r="E21" s="4">
         <v>0.66666666666666663</v>
       </c>
     </row>
@@ -1029,10 +1010,10 @@
       <c r="C22" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D22" s="6">
-        <v>0.25</v>
-      </c>
-      <c r="E22" s="6">
+      <c r="D22" s="4">
+        <v>0.25</v>
+      </c>
+      <c r="E22" s="4">
         <v>0.83333333333333337</v>
       </c>
     </row>
@@ -1046,10 +1027,10 @@
       <c r="C23" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="D23" s="6">
-        <v>0.25</v>
-      </c>
-      <c r="E23" s="6">
+      <c r="D23" s="4">
+        <v>0.25</v>
+      </c>
+      <c r="E23" s="4">
         <v>0.83333333333333337</v>
       </c>
     </row>

</xml_diff>